<commit_message>
Updated Sprint Task Sheet for Week 4
</commit_message>
<xml_diff>
--- a/CMPE 202 - Sample Sprint Task Sheet.xlsx
+++ b/CMPE 202 - Sample Sprint Task Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMPE 202\team202-techninjas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E15E36-6F0F-4C23-A1D3-7C9015B55041}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB47AFB-C643-4CE8-AD93-6622CB27F16F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16464" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,32 +582,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -615,6 +597,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,25 +1054,25 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
@@ -1520,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="88" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="88" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1538,54 +1538,54 @@
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="41"/>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
       <c r="R1" s="41"/>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
       <c r="Y1" s="41"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="36"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="43"/>
     </row>
     <row r="2" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="47" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1674,10 +1674,10 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="43"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="48"/>
       <c r="E3" s="7">
         <v>43192</v>
       </c>
@@ -1765,9 +1765,9 @@
       <c r="AG3" s="9"/>
     </row>
     <row r="4" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11">
         <v>200</v>
@@ -1885,9 +1885,9 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="38"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="10">
         <v>200</v>
       </c>
@@ -1944,71 +1944,71 @@
         <v>105</v>
       </c>
       <c r="R5" s="12">
-        <f>SUM(R6:R20)</f>
+        <f t="shared" ref="R5:Y5" si="2">SUM(R6:R20)</f>
         <v>100</v>
       </c>
       <c r="S5" s="12">
-        <f>SUM(S6:S20)</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="T5" s="12">
-        <f>SUM(T6:T20)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="U5" s="12">
-        <f>SUM(U6:U20)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="V5" s="12">
-        <f>SUM(V6:V20)</f>
+        <f t="shared" si="2"/>
         <v>67</v>
       </c>
       <c r="W5" s="12">
-        <f>SUM(W6:W20)</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="X5" s="12">
-        <f>SUM(X6:X20)</f>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="Y5" s="12">
-        <f>SUM(Y6:Y20)</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Z5" s="12">
-        <f t="shared" ref="R5:AF5" si="2">SUM(Z6:Z15)</f>
-        <v>0</v>
+        <f>SUM(Z6:Z20)</f>
+        <v>45</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(AA6:AA20)</f>
+        <v>40</v>
       </c>
       <c r="AB5" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(AB6:AB20)</f>
+        <v>37</v>
       </c>
       <c r="AC5" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(AC6:AC20)</f>
+        <v>31</v>
       </c>
       <c r="AD5" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(AD6:AD20)</f>
+        <v>27</v>
       </c>
       <c r="AE5" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(AE6:AE20)</f>
+        <v>21</v>
       </c>
       <c r="AF5" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(AF6:AF20)</f>
+        <v>15</v>
       </c>
       <c r="AG5" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="35" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="31" t="s">
@@ -2083,16 +2083,30 @@
       <c r="Y6" s="21">
         <v>0</v>
       </c>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="23"/>
+      <c r="Z6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="31" t="s">
         <v>46</v>
       </c>
@@ -2165,16 +2179,30 @@
       <c r="Y7" s="21">
         <v>0</v>
       </c>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="23"/>
+      <c r="Z7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="31" t="s">
         <v>46</v>
       </c>
@@ -2247,16 +2275,30 @@
       <c r="Y8" s="21">
         <v>0</v>
       </c>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
+      <c r="Z8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="31" t="s">
         <v>46</v>
       </c>
@@ -2329,16 +2371,30 @@
       <c r="Y9" s="21">
         <v>0</v>
       </c>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
+      <c r="Z9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="31" t="s">
         <v>46</v>
       </c>
@@ -2411,16 +2467,30 @@
       <c r="Y10" s="21">
         <v>0</v>
       </c>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="23"/>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="23"/>
+      <c r="Z10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="37" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="31" t="s">
@@ -2495,16 +2565,30 @@
       <c r="Y11" s="21">
         <v>0</v>
       </c>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
+      <c r="Z11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:33" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="31" t="s">
         <v>55</v>
       </c>
@@ -2577,16 +2661,30 @@
       <c r="Y12" s="21">
         <v>0</v>
       </c>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="23"/>
-      <c r="AE12" s="23"/>
-      <c r="AF12" s="23"/>
+      <c r="Z12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:33" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="31" t="s">
         <v>56</v>
       </c>
@@ -2659,16 +2757,30 @@
       <c r="Y13" s="21">
         <v>0</v>
       </c>
-      <c r="Z13" s="22"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="23"/>
-      <c r="AF13" s="23"/>
+      <c r="Z13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="31" t="s">
         <v>57</v>
       </c>
@@ -2741,16 +2853,30 @@
       <c r="Y14" s="21">
         <v>0</v>
       </c>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="23"/>
-      <c r="AD14" s="23"/>
-      <c r="AE14" s="23"/>
-      <c r="AF14" s="23"/>
+      <c r="Z14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="31" t="s">
         <v>58</v>
       </c>
@@ -2823,16 +2949,30 @@
       <c r="Y15" s="21">
         <v>0</v>
       </c>
-      <c r="Z15" s="22"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-      <c r="AE15" s="23"/>
-      <c r="AF15" s="23"/>
+      <c r="Z15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="37" t="s">
         <v>47</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -2904,19 +3044,33 @@
       <c r="X16" s="21">
         <v>12</v>
       </c>
-      <c r="Y16" s="46">
+      <c r="Y16" s="34">
         <v>10</v>
       </c>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="23"/>
+      <c r="Z16" s="22">
+        <v>9</v>
+      </c>
+      <c r="AA16" s="23">
+        <v>8</v>
+      </c>
+      <c r="AB16" s="23">
+        <v>7</v>
+      </c>
+      <c r="AC16" s="23">
+        <v>6</v>
+      </c>
+      <c r="AD16" s="23">
+        <v>6</v>
+      </c>
+      <c r="AE16" s="23">
+        <v>4</v>
+      </c>
+      <c r="AF16" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:32" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="31" t="s">
         <v>48</v>
       </c>
@@ -2986,19 +3140,33 @@
       <c r="X17" s="21">
         <v>11</v>
       </c>
-      <c r="Y17" s="46">
+      <c r="Y17" s="34">
         <v>10</v>
       </c>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23"/>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="23"/>
+      <c r="Z17" s="22">
+        <v>9</v>
+      </c>
+      <c r="AA17" s="23">
+        <v>8</v>
+      </c>
+      <c r="AB17" s="23">
+        <v>8</v>
+      </c>
+      <c r="AC17" s="23">
+        <v>6</v>
+      </c>
+      <c r="AD17" s="23">
+        <v>5</v>
+      </c>
+      <c r="AE17" s="23">
+        <v>4</v>
+      </c>
+      <c r="AF17" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:32" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="31" t="s">
         <v>50</v>
       </c>
@@ -3068,19 +3236,33 @@
       <c r="X18" s="21">
         <v>11</v>
       </c>
-      <c r="Y18" s="46">
+      <c r="Y18" s="34">
         <v>10</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="23"/>
-      <c r="AE18" s="23"/>
-      <c r="AF18" s="23"/>
+      <c r="Z18" s="22">
+        <v>9</v>
+      </c>
+      <c r="AA18" s="23">
+        <v>8</v>
+      </c>
+      <c r="AB18" s="23">
+        <v>7</v>
+      </c>
+      <c r="AC18" s="23">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="23">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="23">
+        <v>4</v>
+      </c>
+      <c r="AF18" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="31" t="s">
         <v>51</v>
       </c>
@@ -3150,19 +3332,33 @@
       <c r="X19" s="21">
         <v>12</v>
       </c>
-      <c r="Y19" s="46">
+      <c r="Y19" s="34">
         <v>10</v>
       </c>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="23"/>
+      <c r="Z19" s="22">
+        <v>9</v>
+      </c>
+      <c r="AA19" s="23">
+        <v>8</v>
+      </c>
+      <c r="AB19" s="23">
+        <v>7</v>
+      </c>
+      <c r="AC19" s="23">
+        <v>7</v>
+      </c>
+      <c r="AD19" s="23">
+        <v>5</v>
+      </c>
+      <c r="AE19" s="23">
+        <v>5</v>
+      </c>
+      <c r="AF19" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="31" t="s">
         <v>52</v>
       </c>
@@ -3232,16 +3428,30 @@
       <c r="X20" s="21">
         <v>11</v>
       </c>
-      <c r="Y20" s="46">
+      <c r="Y20" s="34">
         <v>10</v>
       </c>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="23"/>
-      <c r="AE20" s="23"/>
-      <c r="AF20" s="23"/>
+      <c r="Z20" s="22">
+        <v>9</v>
+      </c>
+      <c r="AA20" s="23">
+        <v>8</v>
+      </c>
+      <c r="AB20" s="23">
+        <v>8</v>
+      </c>
+      <c r="AC20" s="23">
+        <v>6</v>
+      </c>
+      <c r="AD20" s="23">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="23">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="23">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:32" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C21" s="24"/>
@@ -23029,17 +23239,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
     <mergeCell ref="Z1:AF1"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>